<commit_message>
Changed aerofoil databases and code for accessing them code
</commit_message>
<xml_diff>
--- a/data/EPPLER 398.xlsx
+++ b/data/EPPLER 398.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a2f87afe3a2f19d/Documents/2023 DBF/Aerofoil data 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Downloads\ADOT_OO_14_12_2023_1.15_PM\ADOT 2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{119DBE25-3646-407B-AD8A-650A3F4B651D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5E17F3F-BF7D-4B1A-9F99-E0C40DB53119}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798273BE-8189-478B-A01B-512D9ADBE03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="3" xr2:uid="{A33F60C1-12B7-4B07-A94C-BE8E29B43824}"/>
+    <workbookView xWindow="12345" yWindow="6015" windowWidth="19680" windowHeight="16395" xr2:uid="{A33F60C1-12B7-4B07-A94C-BE8E29B43824}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="20">
   <si>
     <t>T.U.</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>30 degrees flap deflection</t>
+  </si>
+  <si>
+    <t>Max_Thickness</t>
   </si>
 </sst>
 </file>
@@ -447,30 +450,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97EFB42-E917-4648-848C-D61BD2C89CBE}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -504,8 +507,11 @@
       <c r="K4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -539,8 +545,11 @@
       <c r="K5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -575,7 +584,7 @@
         <v>-1.0940000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -610,7 +619,7 @@
         <v>-1.01</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -645,7 +654,7 @@
         <v>-0.92400000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -680,7 +689,7 @@
         <v>-0.84499999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -715,7 +724,7 @@
         <v>-0.77300000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -750,7 +759,7 @@
         <v>-0.70299999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -785,7 +794,7 @@
         <v>-0.64300000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -820,7 +829,7 @@
         <v>-0.58299999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -855,7 +864,7 @@
         <v>-0.52300000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -890,7 +899,7 @@
         <v>-0.46600000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -925,7 +934,7 @@
         <v>-0.41599999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -960,7 +969,7 @@
         <v>-0.36399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>-0.32400000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>-0.29199999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -1065,7 +1074,7 @@
         <v>-0.26500000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>-0.24199999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>-0.22500000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>-0.219</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>-0.222</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>-0.24399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -1275,7 +1284,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -1310,7 +1319,7 @@
         <v>-0.432</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -1380,7 +1389,7 @@
         <v>-2.8460000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -1415,7 +1424,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>0.45700000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -1520,7 +1529,7 @@
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -1555,7 +1564,7 @@
         <v>0.30099999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1625,7 +1634,7 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1660,7 +1669,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1765,7 +1774,7 @@
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -1870,7 +1879,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -1905,7 +1914,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -1940,7 +1949,7 @@
         <v>0.38200000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -1975,7 +1984,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -2010,7 +2019,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -2045,7 +2054,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>0.46899999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -2115,7 +2124,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -2150,7 +2159,7 @@
         <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -2185,7 +2194,7 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>0.66200000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -2255,7 +2264,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -2290,7 +2299,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>1.165</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -2465,7 +2474,7 @@
         <v>1.254</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -2500,7 +2509,7 @@
         <v>1.3380000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>1.429</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -2570,7 +2579,7 @@
         <v>1.526</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -2605,7 +2614,7 @@
         <v>1.6140000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -2640,7 +2649,7 @@
         <v>1.726</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -2688,9 +2697,9 @@
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2710,7 +2719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2721,7 +2730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2732,7 +2741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -3035,7 +3044,7 @@
         <v>-2.61</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -3136,7 +3145,7 @@
         <v>-2.5009999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -3237,7 +3246,7 @@
         <v>-2.3839999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>-2.3029999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -3439,7 +3448,7 @@
         <v>-2.254</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -3540,7 +3549,7 @@
         <v>-2.214</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -3641,7 +3650,7 @@
         <v>-2.2069999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>-2.282</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -3843,7 +3852,7 @@
         <v>-2.4569999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -3944,7 +3953,7 @@
         <v>-2.8210000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -4045,7 +4054,7 @@
         <v>-3.6560000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>-6.2720000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -4247,7 +4256,7 @@
         <v>-97.44</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -4348,7 +4357,7 @@
         <v>5.7370000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -4449,7 +4458,7 @@
         <v>2.5840000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>1.6240000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -4651,7 +4660,7 @@
         <v>0.52900000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -4752,7 +4761,7 @@
         <v>0.94799999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>0.80700000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -4954,7 +4963,7 @@
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -5055,7 +5064,7 @@
         <v>0.33700000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -5156,7 +5165,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -5257,7 +5266,7 @@
         <v>0.309</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -5358,7 +5367,7 @@
         <v>0.29299999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -5459,7 +5468,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -5560,7 +5569,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -5661,7 +5670,7 @@
         <v>0.29399999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -5762,7 +5771,7 @@
         <v>0.27300000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -5863,7 +5872,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -5964,7 +5973,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -6065,7 +6074,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -6166,7 +6175,7 @@
         <v>0.312</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>0.45700000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -6368,7 +6377,7 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -6469,7 +6478,7 @@
         <v>0.49399999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -6570,7 +6579,7 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -6671,7 +6680,7 @@
         <v>0.56699999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -6772,7 +6781,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -6873,7 +6882,7 @@
         <v>0.68400000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -6974,7 +6983,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -7075,7 +7084,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -7176,7 +7185,7 @@
         <v>0.96399999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -7277,7 +7286,7 @@
         <v>1.083</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -7378,7 +7387,7 @@
         <v>1.218</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -7479,7 +7488,7 @@
         <v>1.367</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -7580,7 +7589,7 @@
         <v>1.532</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -7681,7 +7690,7 @@
         <v>1.7130000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -7782,7 +7791,7 @@
         <v>1.895</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -7883,7 +7892,7 @@
         <v>2.0910000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -7984,7 +7993,7 @@
         <v>2.2949999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -8085,7 +8094,7 @@
         <v>2.4950000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -8186,7 +8195,7 @@
         <v>2.669</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -8287,7 +8296,7 @@
         <v>2.8210000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -8388,7 +8397,7 @@
         <v>2.972</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -8489,7 +8498,7 @@
         <v>3.1389999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -8590,7 +8599,7 @@
         <v>3.3479999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -8691,7 +8700,7 @@
         <v>3.5390000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -8792,7 +8801,7 @@
         <v>3.7120000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -8893,7 +8902,7 @@
         <v>3.919</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -8994,7 +9003,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -9108,9 +9117,9 @@
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -9130,7 +9139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -9141,7 +9150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9152,7 +9161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9253,7 +9262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -9354,7 +9363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -9455,7 +9464,7 @@
         <v>-3.2349999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -9556,7 +9565,7 @@
         <v>-3.2450000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -9657,7 +9666,7 @@
         <v>-3.3460000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -9758,7 +9767,7 @@
         <v>-3.6269999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -9859,7 +9868,7 @@
         <v>-4.0179999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -9960,7 +9969,7 @@
         <v>-5.1520000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -10061,7 +10070,7 @@
         <v>-8.0609999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -10162,7 +10171,7 @@
         <v>-37.680999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -10263,7 +10272,7 @@
         <v>10.157999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -10364,7 +10373,7 @@
         <v>3.9569999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -10465,7 +10474,7 @@
         <v>2.306</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -10566,7 +10575,7 @@
         <v>1.5780000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -10667,7 +10676,7 @@
         <v>1.1879999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -10768,7 +10777,7 @@
         <v>0.46200000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -10869,7 +10878,7 @@
         <v>0.41099999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -10970,7 +10979,7 @@
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -11071,7 +11080,7 @@
         <v>0.35199999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -11172,7 +11181,7 @@
         <v>0.32900000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -11273,7 +11282,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -11374,7 +11383,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -11475,7 +11484,7 @@
         <v>0.29399999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -11576,7 +11585,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -11677,7 +11686,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -11778,7 +11787,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -11879,7 +11888,7 @@
         <v>0.29799999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -11980,7 +11989,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -12081,7 +12090,7 @@
         <v>0.309</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -12182,7 +12191,7 @@
         <v>0.437</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -12283,7 +12292,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -12384,7 +12393,7 @@
         <v>0.32900000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -12485,7 +12494,7 @@
         <v>0.45700000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -12586,7 +12595,7 @@
         <v>0.47599999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -12687,7 +12696,7 @@
         <v>0.503</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -12788,7 +12797,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -12889,7 +12898,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -12990,7 +12999,7 @@
         <v>0.64200000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -13091,7 +13100,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -13192,7 +13201,7 @@
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -13293,7 +13302,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -13394,7 +13403,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -13495,7 +13504,7 @@
         <v>1.155</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -13596,7 +13605,7 @@
         <v>1.298</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -13697,7 +13706,7 @@
         <v>1.456</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -13798,7 +13807,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -13899,7 +13908,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -14000,7 +14009,7 @@
         <v>2.0259999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -14101,7 +14110,7 @@
         <v>2.2469999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -14202,7 +14211,7 @@
         <v>2.4820000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -14303,7 +14312,7 @@
         <v>2.6829999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -14404,7 +14413,7 @@
         <v>2.8959999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -14505,7 +14514,7 @@
         <v>3.0779999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -14606,7 +14615,7 @@
         <v>3.234</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -14707,7 +14716,7 @@
         <v>3.3879999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -14808,7 +14817,7 @@
         <v>3.5550000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -14909,7 +14918,7 @@
         <v>3.7349999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -15010,7 +15019,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -15111,7 +15120,7 @@
         <v>4.1429999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -15212,7 +15221,7 @@
         <v>4.3470000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -15313,7 +15322,7 @@
         <v>4.5620000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -15414,7 +15423,7 @@
         <v>4.7839999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -15524,13 +15533,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451347CC-00D4-405C-BCDA-BD0021DB897B}">
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -15550,7 +15559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -15561,7 +15570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -15572,7 +15581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -15673,7 +15682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -15774,7 +15783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -15875,7 +15884,7 @@
         <v>-4.3810000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -15976,7 +15985,7 @@
         <v>-5.2110000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -16077,7 +16086,7 @@
         <v>-7.1859999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -16178,7 +16187,7 @@
         <v>-15.327999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -16279,7 +16288,7 @@
         <v>30.882999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -16380,7 +16389,7 @@
         <v>6.3769999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -16481,7 +16490,7 @@
         <v>3.226</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -16582,7 +16591,7 @@
         <v>2.0609999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -16683,7 +16692,7 @@
         <v>1.468</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -16784,7 +16793,7 @@
         <v>1.127</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -16885,7 +16894,7 @@
         <v>0.91600000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -16986,7 +16995,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -17087,7 +17096,7 @@
         <v>0.68899999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -17188,7 +17197,7 @@
         <v>0.629</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -17289,7 +17298,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -17390,7 +17399,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -17491,7 +17500,7 @@
         <v>0.308</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -17592,7 +17601,7 @@
         <v>0.29799999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -17693,7 +17702,7 @@
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -17794,7 +17803,7 @@
         <v>0.47299999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -17895,7 +17904,7 @@
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -17996,7 +18005,7 @@
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -18097,7 +18106,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -18198,7 +18207,7 @@
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -18299,7 +18308,7 @@
         <v>0.30299999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -18400,7 +18409,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -18501,7 +18510,7 @@
         <v>0.317</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -18602,7 +18611,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -18703,7 +18712,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -18804,7 +18813,7 @@
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -18905,7 +18914,7 @@
         <v>0.49399999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -19006,7 +19015,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -19107,7 +19116,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -19208,7 +19217,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -19309,7 +19318,7 @@
         <v>0.69599999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -19410,7 +19419,7 @@
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -19511,7 +19520,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -19612,7 +19621,7 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -19713,7 +19722,7 @@
         <v>1.1379999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -19814,7 +19823,7 @@
         <v>1.2749999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -19915,7 +19924,7 @@
         <v>1.427</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -20016,7 +20025,7 @@
         <v>1.593</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -20117,7 +20126,7 @@
         <v>1.774</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -20218,7 +20227,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -20319,7 +20328,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -20420,7 +20429,7 @@
         <v>2.4039999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -20521,7 +20530,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -20622,7 +20631,7 @@
         <v>2.891</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -20723,7 +20732,7 @@
         <v>3.097</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -20824,7 +20833,7 @@
         <v>3.2669999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -20925,7 +20934,7 @@
         <v>3.3809999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -21026,7 +21035,7 @@
         <v>3.512</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -21127,7 +21136,7 @@
         <v>3.6720000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -21228,7 +21237,7 @@
         <v>3.847</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -21329,7 +21338,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -21430,7 +21439,7 @@
         <v>4.2549999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -21531,7 +21540,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -21632,7 +21641,7 @@
         <v>4.6219999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -21733,7 +21742,7 @@
         <v>4.8029999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -21834,7 +21843,7 @@
         <v>5.0069999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -22164,15 +22173,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9df0515c-157b-471a-a0ef-89af1efb2dd1" xsi:nil="true"/>
@@ -22183,14 +22183,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B033132-A4CC-4373-BF6F-1B377972442C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B033132-A4CC-4373-BF6F-1B377972442C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5f869584-441e-42c5-8d1e-76b11125194b"/>
+    <ds:schemaRef ds:uri="9df0515c-157b-471a-a0ef-89af1efb2dd1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C766254-9259-47E0-B2E7-9C6DB0E52074}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84534FA5-C151-49E2-9A8D-64FB3983379A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9df0515c-157b-471a-a0ef-89af1efb2dd1"/>
+    <ds:schemaRef ds:uri="5f869584-441e-42c5-8d1e-76b11125194b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84534FA5-C151-49E2-9A8D-64FB3983379A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C766254-9259-47E0-B2E7-9C6DB0E52074}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>